<commit_message>
added an object detection sensor that we could use.
</commit_message>
<xml_diff>
--- a/RoboCUP_SSL_Hardware_BOM.xlsx
+++ b/RoboCUP_SSL_Hardware_BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fnl18001\OneDrive - Mälardalens universitet\Robotics_program_university\Ongoing_courses\DVA490\Bill of materials (BOM)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fnl18001\OneDrive - Mälardalens universitet\Robotics_program_university\Ongoing_courses\DVA490\SSL-Hardware-Development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{0478EC04-993D-46B1-9493-DD615EE30C20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{3EFE5E99-CA19-452D-A6B8-E0AB4B51AF5D}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="8_{0478EC04-993D-46B1-9493-DD615EE30C20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{032E53D6-E4CB-4EB8-B236-EC66AFEE40FD}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" activeTab="2" xr2:uid="{DC003E65-EF86-4DD1-BD3D-559D5E22D8BA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" xr2:uid="{DC003E65-EF86-4DD1-BD3D-559D5E22D8BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Complete BOM" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Break Beam BOM" sheetId="4" r:id="rId3"/>
     <sheet name="Encoder BOM" sheetId="5" r:id="rId4"/>
     <sheet name="IMU BOM" sheetId="6" r:id="rId5"/>
-    <sheet name="Active IR (find obstical) BOM" sheetId="7" r:id="rId6"/>
+    <sheet name="Obstical detection BOM" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="35">
   <si>
     <t>Secondary Component</t>
   </si>
@@ -122,6 +122,30 @@
   </si>
   <si>
     <t>Encoder wheel is placed around the shaft and the encoder is placed around the wheel (like a "skivbroms")</t>
+  </si>
+  <si>
+    <t>⁣WSEN-ISDS 6 Axis IMU (Inertial Measurement Unit) &amp; EV-Kits | Sensors | Würth Elektronik Product Catalog (we-online.com)</t>
+  </si>
+  <si>
+    <t>WSEN-ISDS 6 Axis IMU</t>
+  </si>
+  <si>
+    <t>3,0*2,5*0,86</t>
+  </si>
+  <si>
+    <t>Not applicable (sent free of charge by Würth Electronics)</t>
+  </si>
+  <si>
+    <t>OPT8241NBN</t>
+  </si>
+  <si>
+    <t>Data sheet OR url</t>
+  </si>
+  <si>
+    <t>OPT8241NBN Texas Instruments | Mouser Sverige</t>
+  </si>
+  <si>
+    <t>7,9*8,8*0,8</t>
   </si>
 </sst>
 </file>
@@ -531,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F0166DC-E67F-4F2D-87E7-F3AAA07DDA86}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -541,7 +565,7 @@
     <col min="2" max="2" width="31.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="63.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="103.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="43.109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="2" bestFit="1" customWidth="1"/>
   </cols>
@@ -579,13 +603,13 @@
         <f>'Encoder BOM'!B1</f>
         <v>iC-PX2604 + PX01S 26-30</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="3" t="str">
         <f>'IMU BOM'!B1</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="3">
-        <f>'Active IR (find obstical) BOM'!B1</f>
-        <v>0</v>
+        <v>WSEN-ISDS 6 Axis IMU</v>
+      </c>
+      <c r="F2" s="3" t="str">
+        <f>'Obstical detection BOM'!B1</f>
+        <v>OPT8241NBN</v>
       </c>
       <c r="R2">
         <f>P2*Q2</f>
@@ -594,7 +618,7 @@
     </row>
     <row r="3" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="B3" s="3">
         <f>'Communication BOM'!B2</f>
@@ -608,13 +632,13 @@
         <f>'Encoder BOM'!B2</f>
         <v>iC-PX Series - iC-Haus GmbH (ichaus.de)</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="3" t="str">
         <f>'IMU BOM'!B2</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="3">
-        <f>'Active IR (find obstical) BOM'!B2</f>
-        <v>0</v>
+        <v>⁣WSEN-ISDS 6 Axis IMU (Inertial Measurement Unit) &amp; EV-Kits | Sensors | Würth Elektronik Product Catalog (we-online.com)</v>
+      </c>
+      <c r="F3" s="3" t="str">
+        <f>'Obstical detection BOM'!B2</f>
+        <v>OPT8241NBN Texas Instruments | Mouser Sverige</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -633,13 +657,13 @@
         <f>'Encoder BOM'!B3</f>
         <v>(3*3*0,9) samt (Ø26)</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="3" t="str">
         <f>'IMU BOM'!B3</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="3">
-        <f>'Active IR (find obstical) BOM'!B3</f>
-        <v>0</v>
+        <v>3,0*2,5*0,86</v>
+      </c>
+      <c r="F4" s="3" t="str">
+        <f>'Obstical detection BOM'!B3</f>
+        <v>7,9*8,8*0,8</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -660,11 +684,11 @@
       </c>
       <c r="E5" s="3">
         <f>'IMU BOM'!B4</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="3">
-        <f>'Active IR (find obstical) BOM'!B4</f>
-        <v>0</v>
+        <f>'Obstical detection BOM'!B4</f>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -683,13 +707,13 @@
         <f>'Encoder BOM'!B5</f>
         <v>226.4</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="3" t="str">
         <f>'IMU BOM'!B5</f>
-        <v>0</v>
+        <v>Not applicable (sent free of charge by Würth Electronics)</v>
       </c>
       <c r="F6" s="3">
-        <f>'Active IR (find obstical) BOM'!B5</f>
-        <v>0</v>
+        <f>'Obstical detection BOM'!B5</f>
+        <v>605.13</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -708,13 +732,13 @@
         <f>'Encoder BOM'!B6</f>
         <v>679.2</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="3" t="e">
         <f>'IMU BOM'!B6</f>
-        <v>0</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F7" s="3">
-        <f>'Active IR (find obstical) BOM'!B6</f>
-        <v>0</v>
+        <f>'Obstical detection BOM'!B6</f>
+        <v>605.13</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -741,7 +765,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="4">
-        <f>'Active IR (find obstical) BOM'!D1</f>
+        <f>'Obstical detection BOM'!D1</f>
         <v>0</v>
       </c>
     </row>
@@ -766,7 +790,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="4">
-        <f>'Active IR (find obstical) BOM'!D2</f>
+        <f>'Obstical detection BOM'!D2</f>
         <v>0</v>
       </c>
     </row>
@@ -791,7 +815,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="4">
-        <f>'Active IR (find obstical) BOM'!D3</f>
+        <f>'Obstical detection BOM'!D3</f>
         <v>0</v>
       </c>
     </row>
@@ -816,7 +840,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="4">
-        <f>'Active IR (find obstical) BOM'!D4</f>
+        <f>'Obstical detection BOM'!D4</f>
         <v>0</v>
       </c>
     </row>
@@ -841,7 +865,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="4">
-        <f>'Active IR (find obstical) BOM'!D5</f>
+        <f>'Obstical detection BOM'!D5</f>
         <v>0</v>
       </c>
     </row>
@@ -866,7 +890,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="4">
-        <f>'Active IR (find obstical) BOM'!D6</f>
+        <f>'Obstical detection BOM'!D6</f>
         <v>0</v>
       </c>
     </row>
@@ -894,7 +918,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="5">
-        <f>'Active IR (find obstical) BOM'!F1</f>
+        <f>'Obstical detection BOM'!F1</f>
         <v>0</v>
       </c>
     </row>
@@ -919,7 +943,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="5">
-        <f>'Active IR (find obstical) BOM'!F2</f>
+        <f>'Obstical detection BOM'!F2</f>
         <v>0</v>
       </c>
     </row>
@@ -944,7 +968,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="5">
-        <f>'Active IR (find obstical) BOM'!F3</f>
+        <f>'Obstical detection BOM'!F3</f>
         <v>0</v>
       </c>
     </row>
@@ -969,7 +993,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="5">
-        <f>'Active IR (find obstical) BOM'!F4</f>
+        <f>'Obstical detection BOM'!F4</f>
         <v>0</v>
       </c>
     </row>
@@ -994,7 +1018,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="5">
-        <f>'Active IR (find obstical) BOM'!F5</f>
+        <f>'Obstical detection BOM'!F5</f>
         <v>0</v>
       </c>
     </row>
@@ -1019,7 +1043,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="5">
-        <f>'Active IR (find obstical) BOM'!F6</f>
+        <f>'Obstical detection BOM'!F6</f>
         <v>0</v>
       </c>
     </row>
@@ -1146,8 +1170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF50F67-A8F6-49F0-9346-CB66B5F2F9DC}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1234,10 +1258,6 @@
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
-      </c>
-      <c r="B6">
-        <f>B4*B5</f>
-        <v>0</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
@@ -1456,13 +1476,13 @@
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:E6"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="103.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.44140625" bestFit="1" customWidth="1"/>
@@ -1485,6 +1505,9 @@
       <c r="A1" t="s">
         <v>1</v>
       </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -1500,6 +1523,9 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
@@ -1511,6 +1537,9 @@
       <c r="A3" t="s">
         <v>15</v>
       </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
       <c r="C3" t="s">
         <v>15</v>
       </c>
@@ -1522,6 +1551,9 @@
       <c r="A4" t="s">
         <v>13</v>
       </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
@@ -1533,6 +1565,9 @@
       <c r="A5" t="s">
         <v>18</v>
       </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
       <c r="C5" t="s">
         <v>18</v>
       </c>
@@ -1544,9 +1579,9 @@
       <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="e">
         <f>B4*B5</f>
-        <v>0</v>
+        <v>#VALUE!</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
@@ -1564,6 +1599,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" location="2536030320001" display="https://www.we-online.com/en/components/products/WSEN-ISDS?sq=2536030320001 - 2536030320001" xr:uid="{71F8783D-DA3C-4C05-9FE2-53B5EDE0E737}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1573,13 +1611,13 @@
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.44140625" bestFit="1" customWidth="1"/>
@@ -1602,6 +1640,9 @@
       <c r="A1" t="s">
         <v>1</v>
       </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -1615,7 +1656,10 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>32</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -1628,6 +1672,9 @@
       <c r="A3" t="s">
         <v>15</v>
       </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
       <c r="C3" t="s">
         <v>15</v>
       </c>
@@ -1639,6 +1686,9 @@
       <c r="A4" t="s">
         <v>13</v>
       </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
@@ -1650,6 +1700,9 @@
       <c r="A5" t="s">
         <v>18</v>
       </c>
+      <c r="B5">
+        <v>605.13</v>
+      </c>
       <c r="C5" t="s">
         <v>18</v>
       </c>
@@ -1663,7 +1716,7 @@
       </c>
       <c r="B6">
         <f>B4*B5</f>
-        <v>0</v>
+        <v>605.13</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
@@ -1681,6 +1734,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="https://www.mouser.se/ProductDetail/Texas-Instruments/OPT8241NBN?qs=cGEy3R83DS%2FxFMUAL%252BoBvw%3D%3D" xr:uid="{96895479-C619-4399-A80B-8453A68129DF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1694,15 +1750,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009886D6671A81FB4788FD8CEEA40A8F5A" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="58e97b55baf7639b4d456708924fe61d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d249f748-2859-45fd-a747-2e289ca8c4c8" xmlns:ns4="52418e62-0214-4ef5-8ea7-4e8018f8a97c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="209907aae15c3e25da3474742949ee53" ns3:_="" ns4:_="">
     <xsd:import namespace="d249f748-2859-45fd-a747-2e289ca8c4c8"/>
@@ -1935,32 +1982,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4488793-54B9-460A-B96E-16211E37EA37}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="52418e62-0214-4ef5-8ea7-4e8018f8a97c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="52418e62-0214-4ef5-8ea7-4e8018f8a97c"/>
     <ds:schemaRef ds:uri="d249f748-2859-45fd-a747-2e289ca8c4c8"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22116008-86D0-4EEA-B78C-D9F133BB2C6E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEE859D4-628B-41C0-A1A0-E85EDB85793E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1977,4 +2025,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22116008-86D0-4EEA-B78C-D9F133BB2C6E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>